<commit_message>
gem to pedistal adding complete
</commit_message>
<xml_diff>
--- a/LabyrinthExplorer/area3.xlsx
+++ b/LabyrinthExplorer/area3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,15 +11,54 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="9">
+  <si>
+    <t>y2=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x2=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y1=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x1=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Right half</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>SmarPosWall(</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -46,8 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,13 +384,939 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>5000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>4950</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>4950</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>4950</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>4950</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>4950</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>4950</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>4950</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2050</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>2050</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>2300</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2950</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>2950</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>2300</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2050</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>2900</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>2050</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>4900</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2950</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>2900</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>2950</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>4950</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>3400</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>250</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>3400</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>4800</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>3800</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>3650</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>3800</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>4950</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>4150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>2900</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>4150</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>4400</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>4150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>4650</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>4150</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>4950</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>4450</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>2900</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>4450</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>3650</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>4450</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>4000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>4450</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>4950</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>3800</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>3400</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>3800</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>2900</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>3450</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>2850</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>4800</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>2850</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>4800</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2900</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>4800</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>4400</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>4800</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>4600</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>4800</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>4950</v>
+      </c>
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>4950</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>2550</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>4050</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>2550</v>
+      </c>
+      <c r="I21" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>3700</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>2550</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>3700</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>1750</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>4700</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>2250</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>3750</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>2250</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4300</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>2250</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>4300</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>1700</v>
+      </c>
+      <c r="I24" t="s">
+        <v>6</v>
+      </c>
+      <c r="M24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>4950</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>2000</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>4600</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>2000</v>
+      </c>
+      <c r="I25" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>4350</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>1700</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>4950</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>1700</v>
+      </c>
+      <c r="I26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>3700</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>1300</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>3700</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>250</v>
+      </c>
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>3450</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>250</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>3700</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>250</v>
+      </c>
+      <c r="I28" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>3450</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>400</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>3700</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>400</v>
+      </c>
+      <c r="I29" t="s">
+        <v>6</v>
+      </c>
+      <c r="M29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>3750</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>1300</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>4450</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>1300</v>
+      </c>
+      <c r="I30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>